<commit_message>
sheet 2022.07.21 và 2022.07.23 trong file 0.9.Khac phuc HDBK T07.2022 - LK 2022-07-30.xlsx
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/NhatKyGuiEmail/DANH_SACH_NHAT_KY_GUI_EMAIL.xlsx
+++ b/API/wwwroot/docs/NhatKyGuiEmail/DANH_SACH_NHAT_KY_GUI_EMAIL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\bill-back-end\API\wwwroot\docs\NhatKyGuiEmail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pmbk\bills\bill-back-end\API\wwwroot\docs\NhatKyGuiEmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -537,15 +537,14 @@
     <col min="2" max="2" width="22.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="27" style="3" customWidth="1"/>
-    <col min="9" max="9" width="31.33203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="31.88671875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="31" style="3" customWidth="1"/>
-    <col min="13" max="13" width="31.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="31" style="3" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="27" style="3" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="28.109375" style="3" customWidth="1"/>
+    <col min="12" max="13" width="31.88671875" style="3" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -592,28 +591,28 @@
         <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>15</v>
@@ -626,8 +625,8 @@
       <c r="D7" s="13"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>

</xml_diff>